<commit_message>
Add torpedo attack visualization system with convoy support
- Add torpedo_attacks and torpedoes_fired database schema
- Add convoy_ships table for multi-ship convoy attacks
- Create dynamic attack visualization (attack_viz.html)
- Add torpedo attacks selector page (/torpedo_attacks)
- Support bow/stern tube launches with gyro angle handling
- Handle 'down the throat' attack geometry
- Add dynamic scaling for convoy visibility
- Add real-time/10x speed control
- Add Jake (Aichi E13A) aircraft image
- Add ship icons (AKtop.png, cobiatop.png)
- Include attack data for Patrol 1 attacks 1-4
- Update map and viewer with Jake aircraft support
</commit_message>
<xml_diff>
--- a/patrolReports/Cobia_aircraft_contacts.xlsx
+++ b/patrolReports/Cobia_aircraft_contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmkna\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EBB0DA-E506-49CB-9C22-67AE029CA47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587EE81E-35E2-4FA7-862D-23A26E442D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F3686B0-1F77-483D-8FCF-7AD4AF6A6B74}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="76">
   <si>
     <t>patrol</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>Dinah</t>
+  </si>
+  <si>
+    <t>Dropped one bomb at 0756, "shook up the ship considerably"</t>
   </si>
 </sst>
 </file>
@@ -919,9 +922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7CF73-FDB9-42AD-86E0-C70C3B3D7054}">
   <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1455,6 +1458,9 @@
       <c r="R9" t="s">
         <v>31</v>
       </c>
+      <c r="S9" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10">

</xml_diff>